<commit_message>
Update model for 2021
</commit_message>
<xml_diff>
--- a/data/IceAnom.xlsx
+++ b/data/IceAnom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/HSmod/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/Harpseals/HSmodel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{243BB17A-4E6B-47A4-84D4-77C4EA836F85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{5BF52D47-69F3-4069-B9AB-064B4C3E0A2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AE961753-35BE-474E-8549-EFD56D08DF62}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1845" windowWidth="27120" windowHeight="14355" xr2:uid="{09E41039-429D-4452-BBCC-6806428E6920}"/>
+    <workbookView xWindow="-27975" yWindow="825" windowWidth="20640" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -398,22 +399,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8238EC70-EC4C-40A9-8D20-DBE1FBB18840}">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.29296875" customWidth="1"/>
+    <col min="3" max="3" width="11.87890625" customWidth="1"/>
+    <col min="4" max="4" width="11.41015625" customWidth="1"/>
+    <col min="5" max="5" width="10.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +431,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1969</v>
       </c>
@@ -441,15 +442,15 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="D2">
-        <f>(B2-AVERAGE(B$2:B$52))/AVERAGE(B$2:B$52)</f>
-        <v>-0.61652313037601059</v>
+        <f t="shared" ref="D2:E6" si="0">(B2-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>-0.6501873119204078</v>
       </c>
       <c r="E2">
-        <f>(C2-AVERAGE(C$2:C$52))/AVERAGE(C$2:C$52)</f>
-        <v>-0.27376797431243888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-0.34652201659221443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1970</v>
       </c>
@@ -460,15 +461,15 @@
         <v>0.32029999999999997</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D52" si="0">(B3-AVERAGE(B$2:B$52))/AVERAGE(B$2:B$52)</f>
-        <v>1.0127624971618256E-2</v>
+        <f t="shared" si="0"/>
+        <v>-7.8548179082478603E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E52" si="1">(C3-AVERAGE(C$2:C$52))/AVERAGE(C$2:C$52)</f>
-        <v>0.42531934943459426</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0.28253062552398089</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>1971</v>
       </c>
@@ -480,14 +481,14 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.22260181748097765</v>
+        <v>0.11527359823128429</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>0.47782877286053327</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0.3297796463831224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>1972</v>
       </c>
@@ -499,14 +500,14 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.38094760353358009</v>
+        <v>0.25971872505066651</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
-        <v>0.2860358788217226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0.15720059561795344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>1973</v>
       </c>
@@ -518,14 +519,14 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.17736016432309115</v>
+        <v>7.4003561997175005E-2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
-        <v>0.14764239843640936</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.2671396573945452E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>1974</v>
       </c>
@@ -536,15 +537,15 @@
         <v>0.2586</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>0.36263550582681647</v>
+        <f t="shared" ref="D7:D19" si="1">(B7-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>0.2430141865749556</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
-        <v>0.15075736423286326</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E7:E19" si="2">(C7-AVERAGE(C$2:C$33))/AVERAGE(C$2:C$33)</f>
+        <v>3.547430459101307E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>1975</v>
       </c>
@@ -555,15 +556,15 @@
         <v>0.20680000000000001</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0.21344576862759584</v>
+        <f t="shared" si="1"/>
+        <v>0.10692132899342882</v>
       </c>
       <c r="E8">
-        <f t="shared" si="1"/>
-        <v>-7.9750104704732649E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-0.17194088867199722</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>1976</v>
       </c>
@@ -574,15 +575,15 @@
         <v>0.34749999999999998</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0.13750442225542939</v>
+        <f t="shared" si="1"/>
+        <v>3.7646625314745524E-2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
-        <v>0.54635802038252113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.39144362275861183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>1977</v>
       </c>
@@ -593,15 +594,15 @@
         <v>0.2387</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0.24064461963322992</v>
+        <f t="shared" si="1"/>
+        <v>0.13173248172941113</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
-        <v>6.220333659081384E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-4.4208366179911758E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>1978</v>
       </c>
@@ -612,15 +613,15 @@
         <v>0.10539999999999999</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>-7.739343024453095E-2</v>
+        <f t="shared" si="1"/>
+        <v>-0.15838604679727311</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
-        <v>-0.53097515007678353</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-0.57796213571580524</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>1979</v>
       </c>
@@ -631,15 +632,15 @@
         <v>0.26650000000000001</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0.273767972838111</v>
+        <f t="shared" si="1"/>
+        <v>0.16194804397224102</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>0.18591197822141561</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>6.7107123640777269E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>1980</v>
       </c>
@@ -650,15 +651,15 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>3.3287042659583904E-2</v>
+        <f t="shared" si="1"/>
+        <v>-5.7421851010256049E-2</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>0.17033714923914561</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.3092583555438722E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>1981</v>
       </c>
@@ -669,15 +670,15 @@
         <v>0.20979999999999999</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>-0.44121172438920081</v>
+        <f t="shared" si="1"/>
+        <v>-0.49026592151323461</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>-6.6400251291358472E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-0.15992842574170715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>1982</v>
       </c>
@@ -688,15 +689,15 @@
         <v>0.20019999999999999</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>-9.1935390188137331E-2</v>
+        <f t="shared" si="1"/>
+        <v>-0.17165141558680827</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
-        <v>-0.10911978221415616</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-0.19836830711863571</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>1983</v>
       </c>
@@ -707,15 +708,15 @@
         <v>0.28270000000000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>-0.22712175855277414</v>
+        <f t="shared" si="1"/>
+        <v>-0.29497021433396792</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>0.25800118665363669</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.13197442346434418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>1984</v>
       </c>
@@ -726,15 +727,15 @@
         <v>0.3175</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>-2.0033477133639309E-2</v>
+        <f t="shared" si="1"/>
+        <v>-0.1060615365718847</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
-        <v>0.41285948624877838</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.2713189934557102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>1985</v>
       </c>
@@ -745,15 +746,15 @@
         <v>0.2581</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0.15958665772535008</v>
+        <f t="shared" si="1"/>
+        <v>5.7790333476632122E-2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
-        <v>0.14853238866396754</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3.3472227435964709E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>1986</v>
       </c>
@@ -764,15 +765,15 @@
         <v>0.18</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0.24845419071405558</v>
+        <f t="shared" si="1"/>
+        <v>0.13885647607934667</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
-        <v>-0.199008795197543</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>-0.27925222418258955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>1987</v>
       </c>
@@ -783,15 +784,15 @@
         <v>0.17519999999999999</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>7.3950671390779418E-2</v>
+        <f t="shared" ref="D20:D38" si="3">(B20-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>-2.0327949395074561E-2</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
-        <v>-0.22036856065894184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E20:E38" si="4">(C20-AVERAGE(C$2:C$33))/AVERAGE(C$2:C$33)</f>
+        <v>-0.29847216487105382</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>1988</v>
       </c>
@@ -802,15 +803,15 @@
         <v>0.29859999999999998</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0.15877877106181648</v>
+        <f t="shared" si="3"/>
+        <v>5.7053368543880253E-2</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
-        <v>0.32875540974452028</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.19564047699488199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>1989</v>
       </c>
@@ -821,15 +822,15 @@
         <v>0.2263</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0.32762708374035671</v>
+        <f t="shared" si="3"/>
+        <v>0.21107903948903772</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
-        <v>7.0239424822001557E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-9.3859879625111123E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>1990</v>
       </c>
@@ -840,15 +841,15 @@
         <v>0.33839999999999998</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0.3790625346520014</v>
+        <f t="shared" si="3"/>
+        <v>0.25799914020757858</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
-        <v>0.50586346502861912</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.35500581853673163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>1991</v>
       </c>
@@ -859,15 +860,15 @@
         <v>0.28189999999999998</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0.32520342374975564</v>
+        <f t="shared" si="3"/>
+        <v>0.20886814469078185</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
-        <v>0.2544412257434035</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.12877110001626671</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>1992</v>
       </c>
@@ -878,15 +879,15 @@
         <v>0.22409999999999999</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0.34297693034749671</v>
+        <f t="shared" si="3"/>
+        <v>0.22508137321132474</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
-        <v>-2.7659500209410194E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.10266901910732396</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>1993</v>
       </c>
@@ -897,15 +898,15 @@
         <v>0.29039999999999999</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0.43184446333620208</v>
+        <f t="shared" si="3"/>
+        <v>0.30614751581403915</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
-        <v>0.29226581041463062</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.16280641165208889</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>1994</v>
       </c>
@@ -916,15 +917,15 @@
         <v>0.2135</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0.2823854305824704</v>
+        <f t="shared" si="3"/>
+        <v>0.16980900325492859</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
-        <v>-4.9935432081530146E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.14511305479434922</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>1995</v>
       </c>
@@ -935,15 +936,15 @@
         <v>0.24440000000000001</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0.29127218388134085</v>
+        <f t="shared" si="3"/>
+        <v>0.17791561751519996</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
-        <v>8.756805807622503E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-2.1384686612360385E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>1996</v>
       </c>
@@ -954,15 +955,15 @@
         <v>0.31280000000000002</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>-0.30952619823320998</v>
+        <f t="shared" si="3"/>
+        <v>-0.37014063747466674</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
-        <v>0.39194471590115876</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.25249946819825569</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>1997</v>
       </c>
@@ -973,15 +974,15 @@
         <v>0.24529999999999999</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
-        <v>0.1536621555261031</v>
+        <f t="shared" si="3"/>
+        <v>5.2385923969784538E-2</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
-        <v>9.1573014100237243E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-1.7780947733273395E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>1998</v>
       </c>
@@ -992,15 +993,15 @@
         <v>0.1754</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
-        <v>-0.15414266328023116</v>
+        <f t="shared" si="3"/>
+        <v>-0.22839771540870843</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>-0.21947857043138352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.29767133400903445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>1999</v>
       </c>
@@ -1011,15 +1012,15 @@
         <v>0.25480000000000003</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
-        <v>-4.8040214802807131E-2</v>
+        <f t="shared" si="3"/>
+        <v>-0.13160965424061902</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
-        <v>0.13384754990925596</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2.0258518212645637E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>2000</v>
       </c>
@@ -1030,15 +1031,15 @@
         <v>0.21329999999999999</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
-        <v>-0.16168293880654547</v>
+        <f t="shared" si="3"/>
+        <v>-0.2352760547810599</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
-        <v>-5.0825422309088458E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.14591388565636859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>2001</v>
       </c>
@@ -1049,15 +1050,15 @@
         <v>0.1384</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
-        <v>1.7398604943421523E-2</v>
+        <f t="shared" si="3"/>
+        <v>-7.1915494687710968E-2</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
-        <v>-0.38412676252966638</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.44582504348261326</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>2002</v>
       </c>
@@ -1068,15 +1069,15 @@
         <v>0.21560000000000001</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
-        <v>4.271238706747691E-2</v>
+        <f t="shared" si="3"/>
+        <v>-4.8823926794816626E-2</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
-        <v>-4.059053469216807E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.13670433074314603</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>2003</v>
       </c>
@@ -1087,15 +1088,15 @@
         <v>0.1968</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
-        <v>0.23660518631556149</v>
+        <f t="shared" si="3"/>
+        <v>0.12804765706565138</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
-        <v>-0.12424961608264697</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.2119824317729645</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>2004</v>
       </c>
@@ -1106,15 +1107,15 @@
         <v>8.6699999999999999E-2</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
-        <v>7.5027853608824358E-2</v>
+        <f t="shared" si="3"/>
+        <v>-1.9345329484738601E-2</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
-        <v>-0.61418923635348321</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>-0.65283982131461393</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>2005</v>
       </c>
@@ -1125,15 +1126,15 @@
         <v>0.2676</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
-        <v>-1.1416019389280047E-2</v>
+        <f t="shared" si="3"/>
+        <v>-9.8200577289197288E-2</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
-        <v>0.19080692447298614</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.1511693381883623E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>2006</v>
       </c>
@@ -1144,15 +1145,15 @@
         <v>0.1366</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
-        <v>-0.22496739411668423</v>
+        <f t="shared" ref="D39:E44" si="5">(B39-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>-0.29300497451329599</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
-        <v>-0.39213667457769097</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-0.45303252124078736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>2007</v>
       </c>
@@ -1163,15 +1164,15 @@
         <v>9.5399999999999999E-2</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
-        <v>-0.55189219729331573</v>
+        <f t="shared" si="5"/>
+        <v>-0.59123011730025177</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
-        <v>-0.57547466145469772</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-0.61800367881677243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>2008</v>
       </c>
@@ -1182,15 +1183,15 @@
         <v>0.26910000000000001</v>
       </c>
       <c r="D41">
-        <f t="shared" si="0"/>
-        <v>1.3897762734775488E-2</v>
+        <f t="shared" si="5"/>
+        <v>-7.5109009396302814E-2</v>
       </c>
       <c r="E41">
-        <f t="shared" si="1"/>
-        <v>0.19748185117967329</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>7.7517924847028727E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>2009</v>
       </c>
@@ -1201,15 +1202,15 @@
         <v>0.19259999999999999</v>
       </c>
       <c r="D42">
-        <f t="shared" si="0"/>
-        <v>0.14531399333625505</v>
+        <f t="shared" si="5"/>
+        <v>4.4770619664681072E-2</v>
       </c>
       <c r="E42">
-        <f t="shared" si="1"/>
-        <v>-0.14293941086137099</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-0.22879987987537079</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>2010</v>
       </c>
@@ -1220,15 +1221,15 @@
         <v>0.112</v>
       </c>
       <c r="D43">
-        <f t="shared" si="0"/>
-        <v>-0.94560229798873185</v>
+        <f t="shared" si="5"/>
+        <v>-0.95037769452803533</v>
       </c>
       <c r="E43">
-        <f t="shared" si="1"/>
-        <v>-0.5016054725673601</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-0.5515347172691667</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>2011</v>
       </c>
@@ -1239,15 +1240,15 @@
         <v>0.15049999999999999</v>
       </c>
       <c r="D44">
-        <f t="shared" si="0"/>
-        <v>-0.45144495546062746</v>
+        <f t="shared" si="5"/>
+        <v>-0.49960081066142598</v>
       </c>
       <c r="E44">
-        <f t="shared" si="1"/>
-        <v>-0.33028235376239012</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-0.39737477633044288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>2012</v>
       </c>
@@ -1258,15 +1259,15 @@
         <v>0.2147</v>
       </c>
       <c r="D45">
-        <f t="shared" si="0"/>
-        <v>-0.5949794860151123</v>
+        <f t="shared" ref="D45:D47" si="6">(B45-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>-0.63053491371368919</v>
       </c>
       <c r="E45">
-        <f t="shared" si="1"/>
-        <v>-4.4595490716180408E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E45:E47" si="7">(C45-AVERAGE(C$2:C$33))/AVERAGE(C$2:C$33)</f>
+        <v>-0.14030806962223313</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>2013</v>
       </c>
@@ -1277,15 +1278,15 @@
         <v>9.3200000000000005E-2</v>
       </c>
       <c r="D46">
-        <f t="shared" si="0"/>
-        <v>-0.22254373412608314</v>
+        <f t="shared" si="6"/>
+        <v>-0.29079407971504012</v>
       </c>
       <c r="E46">
-        <f t="shared" si="1"/>
-        <v>-0.58526455395783894</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-0.62681281829898516</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>2014</v>
       </c>
@@ -1296,15 +1297,15 @@
         <v>0.23169999999999999</v>
       </c>
       <c r="D47">
-        <f t="shared" si="0"/>
-        <v>0.19674944424789972</v>
+        <f t="shared" si="6"/>
+        <v>9.1690720383221902E-2</v>
       </c>
       <c r="E47">
-        <f t="shared" si="1"/>
-        <v>3.1053678626273815E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-7.223744635058886E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>2015</v>
       </c>
@@ -1315,15 +1316,15 @@
         <v>0.27200000000000002</v>
       </c>
       <c r="D48">
-        <f t="shared" si="0"/>
-        <v>0.14019737780054167</v>
+        <f t="shared" ref="D48:E53" si="8">(B48-AVERAGE(B$2:B$33))/AVERAGE(B$2:B$33)</f>
+        <v>4.0103175090585357E-2</v>
       </c>
       <c r="E48">
-        <f t="shared" si="1"/>
-        <v>0.21038670947926849</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>8.9129972346309275E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>2016</v>
       </c>
@@ -1334,15 +1335,15 @@
         <v>0.2893</v>
       </c>
       <c r="D49">
-        <f t="shared" si="0"/>
-        <v>-0.65907182798878472</v>
+        <f t="shared" si="8"/>
+        <v>-0.68900079837867712</v>
       </c>
       <c r="E49">
-        <f t="shared" si="1"/>
-        <v>0.28737086416306012</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>0.15840184191098255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>2017</v>
       </c>
@@ -1353,15 +1354,15 @@
         <v>0.14050000000000001</v>
       </c>
       <c r="D50">
-        <f t="shared" si="0"/>
-        <v>-0.65099296135344786</v>
+        <f t="shared" si="8"/>
+        <v>-0.68163114905115763</v>
       </c>
       <c r="E50">
-        <f t="shared" si="1"/>
-        <v>-0.37478186514030432</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-0.43741631943141007</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>2018</v>
       </c>
@@ -1372,15 +1373,15 @@
         <v>0.223</v>
       </c>
       <c r="D51">
-        <f t="shared" si="0"/>
-        <v>9.3878542424610384E-2</v>
+        <f t="shared" si="8"/>
+        <v>-2.1494810538597539E-3</v>
       </c>
       <c r="E51">
-        <f t="shared" si="1"/>
-        <v>-7.660896272511545E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-0.10707358884843031</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>2019</v>
       </c>
@@ -1391,15 +1392,35 @@
         <v>0.1434</v>
       </c>
       <c r="D52">
-        <f t="shared" si="0"/>
-        <v>0.27161360840202126</v>
+        <f t="shared" si="8"/>
+        <v>0.15998280415156924</v>
       </c>
       <c r="E52">
-        <f t="shared" si="1"/>
-        <v>-0.36187700684070923</v>
+        <f t="shared" si="8"/>
+        <v>-0.42580427193212961</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A53">
+        <v>2020</v>
+      </c>
+      <c r="B53">
+        <v>0.35970000000000002</v>
+      </c>
+      <c r="C53">
+        <v>0.1862</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="8"/>
+        <v>-0.11637904563041196</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="8"/>
+        <v>-0.25442646745998981</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>